<commit_message>
Tableau link added to readme. Changed ytd name for tableau streamlining.
</commit_message>
<xml_diff>
--- a/documentation/gv_2024_compliance_analysis.xlsx
+++ b/documentation/gv_2024_compliance_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarpy\Documents\portfolio_projects\gv_break_risk_pipeline\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C5FEC4-E212-4736-B480-B05873CEBCE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16FE8A5-D43D-4F46-BC10-A053D7F1E514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{17B12724-4E2C-416B-BEF4-F6D2AE0BDEEB}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>month</t>
   </si>
@@ -123,13 +123,16 @@
   <si>
     <t>Percent</t>
   </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0&quot;%&quot;"/>
+    <numFmt numFmtId="164" formatCode="0.0&quot;%&quot;"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -219,15 +222,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -282,7 +286,7 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Golden Valley Monthly Violation Percent</a:t>
+              <a:t>Golden Valley Overall Monthly Violation Percent</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1157,6 +1161,1395 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Violation Type Pattern of Occurence</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.093044619422574E-2"/>
+          <c:y val="2.3148148148148147E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>missed_lunch</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>116</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0923-468E-B6D4-3ADD3A6FDDB0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>late_lunch_no_waiver</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="90000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="90000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>58</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0923-468E-B6D4-3ADD3A6FDDB0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>late_lunch_waiver</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0923-468E-B6D4-3ADD3A6FDDB0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="599305711"/>
+        <c:axId val="599306191"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="599305711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="599306191"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="599306191"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="120"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Instances</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.5000000000000001E-2"/>
+              <c:y val="0.15028142315543891"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="599305711"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Violation Distribution by</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Month</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="1.8117891513560816E-2"/>
+          <c:y val="4.6296296296296294E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$51</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>missed_lunch</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$52:$B$63</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$52:$C$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>116</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7E0C-4F5F-8AE7-983DE0A288A9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$51</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>late_lunch_no_waiver</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="90000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$52:$B$63</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$52:$D$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>58</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7E0C-4F5F-8AE7-983DE0A288A9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$51</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>late_lunch_waiver</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$52:$B$63</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$52:$E$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7E0C-4F5F-8AE7-983DE0A288A9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="660326943"/>
+        <c:axId val="660324543"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="660326943"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="660324543"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="660324543"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="660326943"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1237,6 +2630,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -2211,6 +3684,1014 @@
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2312,6 +4793,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>746760</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1BCF7F8-050B-4BA6-CAC0-1BEB2D220555}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>632460</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>739140</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1B9434C-80B8-C15D-F1BA-4D601BD47D9C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2637,10 +5190,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020224C2-F1EF-4C73-A841-45A2094DF8EA}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3114,6 +5667,239 @@
       <c r="I14">
         <f t="shared" si="0"/>
         <v>1955</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B51" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52">
+        <v>82</v>
+      </c>
+      <c r="D52">
+        <v>73</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <f>SUM(C52:E52)</f>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53">
+        <v>99</v>
+      </c>
+      <c r="D53">
+        <v>73</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <f t="shared" ref="F53:F63" si="2">SUM(C53:E53)</f>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>10</v>
+      </c>
+      <c r="C54">
+        <v>94</v>
+      </c>
+      <c r="D54">
+        <v>80</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="2"/>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55">
+        <v>104</v>
+      </c>
+      <c r="D55">
+        <v>69</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="2"/>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>12</v>
+      </c>
+      <c r="C56">
+        <v>88</v>
+      </c>
+      <c r="D56">
+        <v>76</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="2"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57">
+        <v>108</v>
+      </c>
+      <c r="D57">
+        <v>64</v>
+      </c>
+      <c r="E57">
+        <v>17</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="2"/>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58">
+        <v>24</v>
+      </c>
+      <c r="D58">
+        <v>82</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="2"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>15</v>
+      </c>
+      <c r="C59">
+        <v>97</v>
+      </c>
+      <c r="D59">
+        <v>67</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="2"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60">
+        <v>101</v>
+      </c>
+      <c r="D60">
+        <v>62</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="2"/>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61">
+        <v>92</v>
+      </c>
+      <c r="D61">
+        <v>71</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="2"/>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>18</v>
+      </c>
+      <c r="C62">
+        <v>98</v>
+      </c>
+      <c r="D62">
+        <v>60</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="2"/>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>19</v>
+      </c>
+      <c r="C63">
+        <v>116</v>
+      </c>
+      <c r="D63">
+        <v>58</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="2"/>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revision on project summary and analysis findings. Clarified insights and company background.
</commit_message>
<xml_diff>
--- a/documentation/gv_2024_compliance_analysis.xlsx
+++ b/documentation/gv_2024_compliance_analysis.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarpy\Documents\portfolio_projects\gv_break_risk_pipeline\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16FE8A5-D43D-4F46-BC10-A053D7F1E514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE332B7-C6A8-4360-9281-66A9AFBB0A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{17B12724-4E2C-416B-BEF4-F6D2AE0BDEEB}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{17B12724-4E2C-416B-BEF4-F6D2AE0BDEEB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DATA" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -222,7 +222,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -231,7 +231,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,7 +529,7 @@
           </c:trendline>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$B$13</c:f>
+              <c:f>DATA!$B$2:$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -574,7 +573,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$13</c:f>
+              <c:f>DATA!$E$2:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>0.0"%"</c:formatCode>
                 <c:ptCount val="12"/>
@@ -882,7 +881,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$M$1</c:f>
+              <c:f>DATA!$M$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -963,7 +962,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$K$2:$K$4</c:f>
+              <c:f>DATA!$K$2:$K$4</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -980,7 +979,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$2:$M$4</c:f>
+              <c:f>DATA!$M$2:$M$4</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1253,7 +1252,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>DATA!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1288,7 +1287,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$B$13</c:f>
+              <c:f>DATA!$B$2:$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -1332,7 +1331,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$13</c:f>
+              <c:f>DATA!$F$2:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1387,7 +1386,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
+              <c:f>DATA!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1428,7 +1427,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$B$13</c:f>
+              <c:f>DATA!$B$2:$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -1472,7 +1471,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$13</c:f>
+              <c:f>DATA!$G$2:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1527,7 +1526,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
+              <c:f>DATA!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1564,7 +1563,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$B$13</c:f>
+              <c:f>DATA!$B$2:$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -1608,7 +1607,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$13</c:f>
+              <c:f>DATA!$H$2:$H$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2005,7 +2004,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$51</c:f>
+              <c:f>DATA!$C$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2026,7 +2025,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$52:$B$63</c:f>
+              <c:f>DATA!$B$52:$B$63</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -2070,7 +2069,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$52:$C$63</c:f>
+              <c:f>DATA!$C$52:$C$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2124,7 +2123,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$51</c:f>
+              <c:f>DATA!$D$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2147,7 +2146,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$52:$B$63</c:f>
+              <c:f>DATA!$B$52:$B$63</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -2191,7 +2190,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$52:$D$63</c:f>
+              <c:f>DATA!$D$52:$D$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2245,7 +2244,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$51</c:f>
+              <c:f>DATA!$E$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2268,7 +2267,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$52:$B$63</c:f>
+              <c:f>DATA!$B$52:$B$63</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -2312,7 +2311,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$52:$E$63</c:f>
+              <c:f>DATA!$E$52:$E$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -5192,8 +5191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020224C2-F1EF-4C73-A841-45A2094DF8EA}">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="H73" sqref="H73"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5638,6 +5637,10 @@
         <f t="shared" si="0"/>
         <v>174</v>
       </c>
+      <c r="K13" s="7">
+        <f>D14/C14</f>
+        <v>0.40476190476190477</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C14">
@@ -5648,9 +5651,9 @@
         <f t="shared" si="1"/>
         <v>1955</v>
       </c>
-      <c r="E14">
-        <f t="shared" si="1"/>
-        <v>487.8</v>
+      <c r="E14" s="5">
+        <f>AVERAGE(E2:E13)</f>
+        <v>40.65</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
@@ -5682,7 +5685,7 @@
       <c r="E51" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F51" s="8" t="s">
+      <c r="F51" s="6" t="s">
         <v>26</v>
       </c>
     </row>
@@ -5908,7 +5911,8 @@
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>